<commit_message>
data-quality-report: Add for list fields.
Add to Web UI and file download
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/project_data_quality_report_public.xlsx
+++ b/indigo/spreadsheetform_guides/project_data_quality_report_public.xlsx
@@ -8,7 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Fields with Single value" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Fields with Multiple Values" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t xml:space="preserve">Field</t>
   </si>
@@ -32,6 +33,15 @@
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:single_fields:count_public_projects_with_public_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projects with at least one data item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:list_fields:field/title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:DOWN:list_fields:count_public_projects_with_at_least_one_public_value</t>
   </si>
 </sst>
 </file>
@@ -46,6 +56,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -67,6 +78,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -144,7 +156,7 @@
   <dimension ref="A7:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7:B7"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -179,4 +191,49 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A9:B10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="40.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.32"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
data-quality-report: Add Introduction to Spreadsheet
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/project_data_quality_report_public.xlsx
+++ b/indigo/spreadsheetform_guides/project_data_quality_report_public.xlsx
@@ -21,7 +21,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+  <si>
+    <t xml:space="preserve">This is our data completeness report. 
+The first tab has data for all fields with a single value, and the second tab has data for fields that accept multiple values. 
+In the first tab, column A has a list of Impact Bond Dataset variables and column B counts how many projects have values for those variables. 
+In the second tab, column A has a list of Impact Bond Dataset variables and column B counts how many projects have at least one value for those variables. 
+These tables are updated once a day.</t>
+  </si>
   <si>
     <t xml:space="preserve">Field</t>
   </si>
@@ -123,9 +130,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -153,7 +164,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A7:B8"/>
+  <dimension ref="A2:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -166,20 +177,25 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
+    <row r="2" customFormat="false" ht="122.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -212,19 +228,19 @@
   </cols>
   <sheetData>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>4</v>
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>